<commit_message>
Added master BOM.  Minor mods to JLCBPB specific BOMs.
</commit_message>
<xml_diff>
--- a/comm_v0p5/production/rev1/BOM_JLCPCB_comm_v0p5_rev1.xlsx
+++ b/comm_v0p5/production/rev1/BOM_JLCPCB_comm_v0p5_rev1.xlsx
@@ -31,50 +31,7 @@
     <t xml:space="preserve">Footprint</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">LCSC Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">（</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">optional</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="0"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
+    <t xml:space="preserve">LCSC Part #</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
@@ -199,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,14 +199,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
       <family val="0"/>
       <charset val="134"/>
     </font>
@@ -428,7 +377,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>